<commit_message>
upload shiny new figures and tables
</commit_message>
<xml_diff>
--- a/Figures/MS/gam_stat_table_YSL_ice_off_formatted.xlsx
+++ b/Figures/MS/gam_stat_table_YSL_ice_off_formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://o365coloradoedu-my.sharepoint.com/personal/isol5015_colorado_edu/Documents/Research/Data/R/NC_YSL_Ice_Phenology/Figures/MS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{99E51E45-1149-8640-9A62-F8FE480CFD0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A5A5BBF1-440E-224F-B219-BF366396E2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42140" yWindow="500" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="-31520" yWindow="2960" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="gam_stat_table_YSL_ice_off" sheetId="1" r:id="rId1"/>
@@ -75,9 +75,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
-    <numFmt numFmtId="174" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="173" formatCode="0.0%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -215,7 +215,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,12 +393,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -563,24 +557,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="33" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -940,14 +922,10 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24:F26"/>
+      <selection activeCell="B23" sqref="B20:F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -985,26 +963,26 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4">
-        <v>1.0000672442356</v>
-      </c>
-      <c r="D2" s="4">
-        <v>1.00012978146397</v>
-      </c>
-      <c r="E2" s="4">
-        <v>20.480047187641102</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2.62032009819002E-5</v>
-      </c>
-      <c r="G2" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H2" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I2" s="14">
-        <v>503.860309730891</v>
+      <c r="C2" s="2">
+        <v>1.00035823438942</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0006885072277201</v>
+      </c>
+      <c r="E2" s="2">
+        <v>14.285938074207801</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3.3926107000220498E-4</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I2" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1014,26 +992,26 @@
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4">
-        <v>1.0001279689111799</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.0002483240187201</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1.2074363259466101</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0.27584988151802398</v>
-      </c>
-      <c r="G3" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H3" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I3" s="14">
-        <v>503.860309730891</v>
+      <c r="C3" s="2">
+        <v>1.0001062597194801</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.00020545351468</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.1582268532456199</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.28577702444217301</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H3" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I3" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1043,26 +1021,26 @@
       <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4">
-        <v>1.00014967285039</v>
-      </c>
-      <c r="D4" s="4">
-        <v>1.0002896938721599</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.57541519270522301</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.45086952638357503</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H4" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I4" s="14">
-        <v>503.860309730891</v>
+      <c r="C4" s="2">
+        <v>1.0001230811220601</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.0002391559766</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5.8839799846233699E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.80927753845050499</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I4" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1072,26 +1050,26 @@
       <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="4">
-        <v>1.1953953831985999</v>
-      </c>
-      <c r="D5" s="4">
-        <v>1.3627098039721199</v>
-      </c>
-      <c r="E5" s="4">
-        <v>9.8634250748705696</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3.1074274552179699E-3</v>
-      </c>
-      <c r="G5" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H5" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I5" s="14">
-        <v>503.860309730891</v>
+      <c r="C5" s="2">
+        <v>1.01048205810309</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.02068826447106</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.4421182511612702</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3.0994191110298398E-3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I5" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1101,26 +1079,26 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="4">
-        <v>2.3544064254091399</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2.9621397205740299</v>
-      </c>
-      <c r="E6" s="4">
-        <v>2.2734716477175301</v>
-      </c>
-      <c r="F6" s="6">
-        <v>8.6535477245135994E-2</v>
-      </c>
-      <c r="G6" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H6" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I6" s="14">
-        <v>503.860309730891</v>
+      <c r="C6" s="2">
+        <v>1.99070830687168</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.51101606891338</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2.0409296908322099</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.108769448510201</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I6" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1130,26 +1108,26 @@
       <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4">
-        <v>1.3658172733962901</v>
-      </c>
-      <c r="D7" s="4">
-        <v>1.6463555028565899</v>
-      </c>
-      <c r="E7" s="4">
-        <v>1.3479625697081801</v>
-      </c>
-      <c r="F7" s="6">
-        <v>0.36212093069482498</v>
-      </c>
-      <c r="G7" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H7" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I7" s="14">
-        <v>503.860309730891</v>
+      <c r="C7" s="2">
+        <v>1.9122077427689399</v>
+      </c>
+      <c r="D7" s="2">
+        <v>2.4163525553799001</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.89698344434921895</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.37159750823043503</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I7" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1159,26 +1137,26 @@
       <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.00001187116353</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.0000234950799001</v>
-      </c>
-      <c r="E8" s="8">
-        <v>9.2274092774436697E-2</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0.76227911737161103</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0.64020544690832404</v>
-      </c>
-      <c r="H8" s="13">
-        <v>-239.958258543608</v>
-      </c>
-      <c r="I8" s="14">
-        <v>503.860309730891</v>
+      <c r="C8" s="2">
+        <v>1.0000881293283399</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0001750595185801</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6.4870485400142106E-2</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.79992210130624397</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.63564914484578094</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-234.51117292974101</v>
+      </c>
+      <c r="I8" s="4">
+        <v>492.92107598948598</v>
       </c>
     </row>
     <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1188,26 +1166,26 @@
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4">
-        <v>1.00000899977182</v>
-      </c>
-      <c r="D9" s="4">
-        <v>1.0000173798187</v>
-      </c>
-      <c r="E9" s="4">
-        <v>19.926997080272901</v>
-      </c>
-      <c r="F9" s="2">
-        <v>3.1520016261388201E-5</v>
-      </c>
-      <c r="G9" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H9" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I9" s="14">
-        <v>509.10421755907799</v>
+      <c r="C9" s="2">
+        <v>1.00093282659775</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.00180390084051</v>
+      </c>
+      <c r="E9" s="2">
+        <v>13.7735005972678</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4.1485665337137601E-4</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H9" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I9" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1217,26 +1195,26 @@
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="4">
-        <v>1.0000926397538701</v>
-      </c>
-      <c r="D10" s="4">
-        <v>1.0001788605705899</v>
-      </c>
-      <c r="E10" s="4">
-        <v>7.1484520305743597</v>
-      </c>
-      <c r="F10" s="6">
-        <v>9.3846544824878197E-3</v>
-      </c>
-      <c r="G10" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H10" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I10" s="14">
-        <v>509.10421755907799</v>
+      <c r="C10" s="2">
+        <v>1.0000701406082</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.0001356948309199</v>
+      </c>
+      <c r="E10" s="2">
+        <v>6.4504869636788396</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1.3381271092969899E-2</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I10" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1246,26 +1224,26 @@
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="4">
-        <v>1.0002142519823201</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.00041344444652</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.93852468645399001</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.33613191589483699</v>
-      </c>
-      <c r="G11" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H11" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I11" s="14">
-        <v>509.10421755907799</v>
+      <c r="C11" s="2">
+        <v>1.00004586755355</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0000889946831599</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.13289103183197001</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.71662763405794105</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I11" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1275,26 +1253,26 @@
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="4">
-        <v>1.2558080970391901</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.4647215316686</v>
-      </c>
-      <c r="E12" s="4">
-        <v>9.2051139322784099</v>
-      </c>
-      <c r="F12" s="6">
-        <v>4.4154278753012997E-3</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H12" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I12" s="14">
-        <v>509.10421755907799</v>
+      <c r="C12" s="2">
+        <v>1.05830783218717</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1.11312769930989</v>
+      </c>
+      <c r="E12" s="2">
+        <v>8.8290380106951307</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4.3285006729696304E-3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H12" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I12" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1304,26 +1282,26 @@
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4">
-        <v>2.3401356251302099</v>
-      </c>
-      <c r="D13" s="4">
-        <v>2.9464957445550799</v>
-      </c>
-      <c r="E13" s="4">
-        <v>2.79965124006615</v>
-      </c>
-      <c r="F13" s="2">
-        <v>4.6775590140920198E-2</v>
-      </c>
-      <c r="G13" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H13" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I13" s="14">
-        <v>509.10421755907799</v>
+      <c r="C13" s="2">
+        <v>1.98482362106737</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2.5051830366340702</v>
+      </c>
+      <c r="E13" s="2">
+        <v>2.7371693107992598</v>
+      </c>
+      <c r="F13" s="1">
+        <v>5.2832996924435098E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I13" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1333,26 +1311,26 @@
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="4">
-        <v>1.56237543845966</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1.94014815794245</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.62536815210199</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.25798142345738101</v>
-      </c>
-      <c r="G14" s="11">
-        <v>0.64079969067540798</v>
-      </c>
-      <c r="H14" s="13">
-        <v>-243.20013366053701</v>
-      </c>
-      <c r="I14" s="14">
-        <v>509.10421755907799</v>
+      <c r="C14" s="2">
+        <v>2.0259996572901402</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2.5611481819724502</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.1299625620653699</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.27724417273450203</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.64031605756054299</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-237.493757256083</v>
+      </c>
+      <c r="I14" s="4">
+        <v>497.35048952870801</v>
       </c>
     </row>
     <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1362,26 +1340,26 @@
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
-        <v>1.0000858029509601</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1.0001655716009501</v>
-      </c>
-      <c r="E15" s="4">
-        <v>19.418502648276299</v>
-      </c>
-      <c r="F15" s="2">
-        <v>3.80307088387876E-5</v>
-      </c>
-      <c r="G15" s="11">
-        <v>0.63675730094764305</v>
-      </c>
-      <c r="H15" s="13">
-        <v>-243.57363831498199</v>
-      </c>
-      <c r="I15" s="14">
-        <v>508.20597262278801</v>
+      <c r="C15" s="2">
+        <v>1.0010126652717699</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.00195848322292</v>
+      </c>
+      <c r="E15" s="2">
+        <v>14.4673852684842</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3.02548054421314E-4</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.64023077834702102</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-237.44442396245699</v>
+      </c>
+      <c r="I15" s="4">
+        <v>495.50475290961703</v>
       </c>
     </row>
     <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1391,26 +1369,26 @@
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4">
-        <v>1.0001653759576701</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1.00031883736898</v>
-      </c>
-      <c r="E16" s="4">
-        <v>6.3152079978823599</v>
-      </c>
-      <c r="F16" s="2">
-        <v>1.43064420874133E-2</v>
-      </c>
-      <c r="G16" s="11">
-        <v>0.63675730094764305</v>
-      </c>
-      <c r="H16" s="13">
-        <v>-243.57363831498199</v>
-      </c>
-      <c r="I16" s="14">
-        <v>508.20597262278801</v>
+      <c r="C16" s="2">
+        <v>1.0000809397319601</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.00015667058832</v>
+      </c>
+      <c r="E16" s="2">
+        <v>7.4098424777601801</v>
+      </c>
+      <c r="F16" s="1">
+        <v>8.2047777289563292E-3</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.64023077834702102</v>
+      </c>
+      <c r="H16" s="4">
+        <v>-237.44442396245699</v>
+      </c>
+      <c r="I16" s="4">
+        <v>495.50475290961703</v>
       </c>
     </row>
     <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1420,26 +1398,26 @@
       <c r="B17" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="4">
-        <v>1.3498596556374101</v>
-      </c>
-      <c r="D17" s="4">
-        <v>1.6162332769499701</v>
-      </c>
-      <c r="E17" s="4">
-        <v>9.2586089606178792</v>
-      </c>
-      <c r="F17" s="6">
-        <v>4.2963050701359503E-3</v>
-      </c>
-      <c r="G17" s="11">
-        <v>0.63675730094764305</v>
-      </c>
-      <c r="H17" s="13">
-        <v>-243.57363831498199</v>
-      </c>
-      <c r="I17" s="14">
-        <v>508.20597262278801</v>
+      <c r="C17" s="2">
+        <v>1.1122540289684699</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.21375079391763</v>
+      </c>
+      <c r="E17" s="2">
+        <v>11.3417530577515</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1.38144174469373E-3</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.64023077834702102</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-237.44442396245699</v>
+      </c>
+      <c r="I17" s="4">
+        <v>495.50475290961703</v>
       </c>
     </row>
     <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1449,26 +1427,26 @@
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="4">
-        <v>2.27360812022861</v>
-      </c>
-      <c r="D18" s="4">
-        <v>2.8720886599464301</v>
-      </c>
-      <c r="E18" s="8">
-        <v>2.68862340998264</v>
-      </c>
-      <c r="F18" s="6">
-        <v>5.4359119333635797E-2</v>
-      </c>
-      <c r="G18" s="11">
-        <v>0.63675730094764305</v>
-      </c>
-      <c r="H18" s="13">
-        <v>-243.57363831498199</v>
-      </c>
-      <c r="I18" s="14">
-        <v>508.20597262278801</v>
+      <c r="C18" s="2">
+        <v>1.97560165188632</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.4988011764598199</v>
+      </c>
+      <c r="E18" s="2">
+        <v>2.7154176492340598</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5.4067934042548997E-2</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.64023077834702102</v>
+      </c>
+      <c r="H18" s="4">
+        <v>-237.44442396245699</v>
+      </c>
+      <c r="I18" s="4">
+        <v>495.50475290961703</v>
       </c>
     </row>
     <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
@@ -1478,142 +1456,142 @@
       <c r="B19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="4">
-        <v>1.63418790545968</v>
-      </c>
-      <c r="D19" s="4">
-        <v>2.0405416505449399</v>
-      </c>
-      <c r="E19" s="4">
-        <v>1.0236804310495999</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.352911779812003</v>
-      </c>
-      <c r="G19" s="11">
-        <v>0.63675730094764305</v>
-      </c>
-      <c r="H19" s="13">
-        <v>-243.57363831498199</v>
-      </c>
-      <c r="I19" s="14">
-        <v>508.20597262278801</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="C19" s="2">
+        <v>2.0517457888063002</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2.5932853681622201</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.10453950663037</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.28482154819018701</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.64023077834702102</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-237.44442396245699</v>
+      </c>
+      <c r="I19" s="4">
+        <v>495.50475290961703</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>4</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="5">
-        <v>1.0000195831397201</v>
-      </c>
-      <c r="D20" s="5">
-        <v>1.00003867180978</v>
-      </c>
-      <c r="E20" s="5">
-        <v>19.1368450641321</v>
-      </c>
-      <c r="F20" s="3">
-        <v>4.0806497862755303E-5</v>
-      </c>
-      <c r="G20" s="12">
-        <v>0.61439976618028902</v>
-      </c>
-      <c r="H20" s="15">
-        <v>-248.590259005641</v>
-      </c>
-      <c r="I20" s="16">
-        <v>512.847713372577</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="C20" s="2">
+        <v>1.0000611343891599</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.00011880034898</v>
+      </c>
+      <c r="E20" s="2">
+        <v>13.4067781872415</v>
+      </c>
+      <c r="F20" s="1">
+        <v>4.7533118481724002E-4</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.61671092869654998</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-242.51041549706099</v>
+      </c>
+      <c r="I20" s="4">
+        <v>501.53261589238701</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>4</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="5">
-        <v>1.0001248972696799</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1.0002484216696499</v>
-      </c>
-      <c r="E21" s="9">
-        <v>5.9045611941385898</v>
-      </c>
-      <c r="F21" s="7">
-        <v>1.7594160329984499E-2</v>
-      </c>
-      <c r="G21" s="12">
-        <v>0.61439976618028902</v>
-      </c>
-      <c r="H21" s="15">
-        <v>-248.590259005641</v>
-      </c>
-      <c r="I21" s="16">
-        <v>512.847713372577</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="C21" s="2">
+        <v>1.37094093502854</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1.6592575836896899</v>
+      </c>
+      <c r="E21" s="2">
+        <v>6.5264075382697699</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1.02096279504431E-2</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.61671092869654998</v>
+      </c>
+      <c r="H21" s="4">
+        <v>-242.51041549706099</v>
+      </c>
+      <c r="I21" s="4">
+        <v>501.53261589238701</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5">
-        <v>1.00081253460317</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1.00161631329312</v>
-      </c>
-      <c r="E22" s="9">
-        <v>9.9405923851137992</v>
-      </c>
-      <c r="F22" s="7">
-        <v>2.3587205228725499E-3</v>
-      </c>
-      <c r="G22" s="12">
-        <v>0.61439976618028902</v>
-      </c>
-      <c r="H22" s="15">
-        <v>-248.590259005641</v>
-      </c>
-      <c r="I22" s="16">
-        <v>512.847713372577</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="C22" s="2">
+        <v>1.0014835557047701</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1.0029350241572099</v>
+      </c>
+      <c r="E22" s="2">
+        <v>9.7498651043430602</v>
+      </c>
+      <c r="F22" s="1">
+        <v>2.5840565182258502E-3</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.61671092869654998</v>
+      </c>
+      <c r="H22" s="4">
+        <v>-242.51041549706099</v>
+      </c>
+      <c r="I22" s="4">
+        <v>501.53261589238701</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>4</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5">
-        <v>2.23020578228618</v>
-      </c>
-      <c r="D23" s="5">
-        <v>2.8316942738751698</v>
-      </c>
-      <c r="E23" s="5">
-        <v>2.6381978621495099</v>
-      </c>
-      <c r="F23" s="7">
-        <v>5.3902047551298703E-2</v>
-      </c>
-      <c r="G23" s="12">
-        <v>0.61439976618028902</v>
-      </c>
-      <c r="H23" s="15">
-        <v>-248.590259005641</v>
-      </c>
-      <c r="I23" s="16">
-        <v>512.847713372577</v>
+      <c r="C23" s="2">
+        <v>2.0439766811093798</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2.5935810409363902</v>
+      </c>
+      <c r="E23" s="2">
+        <v>2.5657906489405198</v>
+      </c>
+      <c r="F23" s="1">
+        <v>5.6123126749309797E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.61671092869654998</v>
+      </c>
+      <c r="H23" s="4">
+        <v>-242.51041549706099</v>
+      </c>
+      <c r="I23" s="4">
+        <v>501.53261589238701</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1623,26 +1601,26 @@
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="4">
-        <v>5.0640717025100201</v>
-      </c>
-      <c r="D24" s="4">
-        <v>6.1850649805092397</v>
-      </c>
-      <c r="E24" s="4">
-        <v>6.1212317521242801</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2.8246014778354701E-5</v>
-      </c>
-      <c r="G24" s="11">
-        <v>0.639409939188198</v>
-      </c>
-      <c r="H24" s="13">
-        <v>-246.08378223510499</v>
-      </c>
-      <c r="I24" s="14">
-        <v>513.57455326958495</v>
+      <c r="C24" s="2">
+        <v>5.5687900940818604</v>
+      </c>
+      <c r="D24" s="2">
+        <v>6.7168341002333802</v>
+      </c>
+      <c r="E24" s="2">
+        <v>4.9461355191820999</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1.85585742659144E-4</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.660629630412498</v>
+      </c>
+      <c r="H24" s="4">
+        <v>-237.930263692322</v>
+      </c>
+      <c r="I24" s="4">
+        <v>500.04038818104902</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1652,26 +1630,26 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="4">
-        <v>1.0010700744096399</v>
-      </c>
-      <c r="D25" s="4">
-        <v>1.00208275529975</v>
-      </c>
-      <c r="E25" s="4">
-        <v>4.9119053338716903</v>
-      </c>
-      <c r="F25" s="2">
-        <v>2.9915851090562901E-2</v>
-      </c>
-      <c r="G25" s="11">
-        <v>0.639409939188198</v>
-      </c>
-      <c r="H25" s="13">
-        <v>-246.08378223510499</v>
-      </c>
-      <c r="I25" s="14">
-        <v>513.57455326958495</v>
+      <c r="C25" s="2">
+        <v>1.5589529317537001</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.9280734021658501</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5.5122082520414297</v>
+      </c>
+      <c r="F25" s="1">
+        <v>9.77695167439252E-3</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.660629630412498</v>
+      </c>
+      <c r="H25" s="4">
+        <v>-237.930263692322</v>
+      </c>
+      <c r="I25" s="4">
+        <v>500.04038818104902</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1681,26 +1659,26 @@
       <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="4">
-        <v>1.2836874737888699</v>
-      </c>
-      <c r="D26" s="4">
-        <v>1.5163466638782399</v>
-      </c>
-      <c r="E26" s="4">
-        <v>9.76154771505451</v>
-      </c>
-      <c r="F26" s="6">
-        <v>4.0460152754543399E-3</v>
-      </c>
-      <c r="G26" s="11">
-        <v>0.639409939188198</v>
-      </c>
-      <c r="H26" s="13">
-        <v>-246.08378223510499</v>
-      </c>
-      <c r="I26" s="14">
-        <v>513.57455326958495</v>
+      <c r="C26" s="2">
+        <v>1.2434071240581599</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.4450228958029301</v>
+      </c>
+      <c r="E26" s="2">
+        <v>10.334540744681201</v>
+      </c>
+      <c r="F26" s="1">
+        <v>3.00243067747385E-3</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.660629630412498</v>
+      </c>
+      <c r="H26" s="4">
+        <v>-237.930263692322</v>
+      </c>
+      <c r="I26" s="4">
+        <v>500.04038818104902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>